<commit_message>
Enviando o Python completo - Pythonv2
</commit_message>
<xml_diff>
--- a/Documentação/Documentação ALL/6tracker - BacklogRequisitos.xlsx
+++ b/Documentação/Documentação ALL/6tracker - BacklogRequisitos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\6Tracker\6tracker\Site\Documentação\Documentação ALL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isabe\OneDrive\Área de Trabalho\6trackerbackup\SixTracker\Documentação\Documentação ALL\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -652,23 +652,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -958,8 +958,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="G2:R62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N62" sqref="N62"/>
+    <sheetView tabSelected="1" topLeftCell="C55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K56" sqref="K56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -974,20 +974,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="7:18" x14ac:dyDescent="0.25">
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
       <c r="M2" s="12"/>
       <c r="N2" s="12"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="10"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="13"/>
     </row>
     <row r="3" spans="7:18" ht="30" x14ac:dyDescent="0.25">
       <c r="G3" s="1" t="s">
@@ -1014,7 +1014,7 @@
       <c r="N3" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="O3" s="11"/>
+      <c r="O3" s="8"/>
     </row>
     <row r="4" spans="7:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G4" s="2">
@@ -2501,7 +2501,7 @@
       </c>
     </row>
     <row r="62" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="N62" s="13"/>
+      <c r="N62" s="9"/>
     </row>
   </sheetData>
   <autoFilter ref="G3:L45">

</xml_diff>